<commit_message>
Fix bug test data1
</commit_message>
<xml_diff>
--- a/src/main/java/resources/testData/TestData.xlsx
+++ b/src/main/java/resources/testData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsingh\git_project\ECP_VW\src\main\java\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsingh\Frameworks\Selenium_ECP_VW\src\main\java\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="client" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="client" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
   <si>
     <t>data1</t>
   </si>
@@ -181,6 +182,66 @@
   </si>
   <si>
     <t>PART_CUST_ADMIN3</t>
+  </si>
+  <si>
+    <t>EMP_Admin</t>
+  </si>
+  <si>
+    <t>Abcd@1234</t>
+  </si>
+  <si>
+    <t>Empirix/Admin</t>
+  </si>
+  <si>
+    <t>Empirix/BusnessAnalyst</t>
+  </si>
+  <si>
+    <t>EMP_Bus_Ana</t>
+  </si>
+  <si>
+    <t>PARTNER/Customer_Admin</t>
+  </si>
+  <si>
+    <t>Part_CustAdmin</t>
+  </si>
+  <si>
+    <t>Part_Devloper</t>
+  </si>
+  <si>
+    <t>PART_EnhUser</t>
+  </si>
+  <si>
+    <t>Part_User1</t>
+  </si>
+  <si>
+    <t>PartClient_CustAdmin</t>
+  </si>
+  <si>
+    <t>PartClient_Dev</t>
+  </si>
+  <si>
+    <t>PartClient_EnhUser</t>
+  </si>
+  <si>
+    <t>PartClient_User</t>
+  </si>
+  <si>
+    <t>Client_CustAdmin</t>
+  </si>
+  <si>
+    <t>Clinet/Customer_Admin</t>
+  </si>
+  <si>
+    <t>Client_Dev</t>
+  </si>
+  <si>
+    <t>Client_EnhUser</t>
+  </si>
+  <si>
+    <t>Clinet/Developer</t>
+  </si>
+  <si>
+    <t>Clinet/Client_EnhUser</t>
   </si>
 </sst>
 </file>
@@ -509,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,6 +581,196 @@
     <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="C3" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -660,7 +911,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>

</xml_diff>